<commit_message>
Confusion Matrix Excel File
</commit_message>
<xml_diff>
--- a/Resources/Confusion Matrix/Confusion Matrix Numbers.xlsx
+++ b/Resources/Confusion Matrix/Confusion Matrix Numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emadsoheili/DA/GitHub/CapstoneProject-UofT-VehicleCrossSellPrediction/Resources/Confusion Matrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAD46A9-3BDD-5149-B3DB-D60C63D5D9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7E7903-329C-E345-80B1-53276A3B309E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{11C484A1-B4B5-8F45-8F72-CC3DC732B263}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="25700" windowHeight="16860" xr2:uid="{11C484A1-B4B5-8F45-8F72-CC3DC732B263}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
     <t>Won't Purchase</t>
   </si>
   <si>
-    <t>Purchase</t>
+    <t>Will Purchase</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>